<commit_message>
Add more change on document
</commit_message>
<xml_diff>
--- a/docs/StoredVariableList.xlsx
+++ b/docs/StoredVariableList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitRepo\idep\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD9C6C3B-7AD0-4A4D-A64E-B40FFC85DC0D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27BC6165-11AA-4940-82BB-D84D81186282}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="37755" yWindow="6840" windowWidth="27000" windowHeight="14265" xr2:uid="{026807F2-CD40-4E39-BF42-D7478ABC8AA8}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Variable Name</t>
   </si>
@@ -48,6 +48,15 @@
   </si>
   <si>
     <t>Store which data source user selected</t>
+  </si>
+  <si>
+    <t>GSEID</t>
+  </si>
+  <si>
+    <t>sting</t>
+  </si>
+  <si>
+    <t>Store GSEID which used as data. Only useful when DataSourse == "Public"</t>
   </si>
 </sst>
 </file>
@@ -428,10 +437,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE139667-7176-406A-93D2-B836CE61A0C4}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -463,6 +472,169 @@
         <v>5</v>
       </c>
     </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="1"/>
+      <c r="B4" s="2"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="1"/>
+      <c r="B5" s="2"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="1"/>
+      <c r="B6" s="2"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="1"/>
+      <c r="B7" s="2"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="1"/>
+      <c r="B8" s="2"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="1"/>
+      <c r="B9" s="2"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="1"/>
+      <c r="B10" s="2"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="1"/>
+      <c r="B11" s="2"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="1"/>
+      <c r="B12" s="2"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="1"/>
+      <c r="B13" s="2"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="1"/>
+      <c r="B14" s="2"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="1"/>
+      <c r="B15" s="2"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="1"/>
+      <c r="B16" s="2"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="1"/>
+      <c r="B17" s="2"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="1"/>
+      <c r="B18" s="2"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="1"/>
+      <c r="B19" s="2"/>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="1"/>
+      <c r="B20" s="2"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="1"/>
+      <c r="B21" s="2"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" s="1"/>
+      <c r="B22" s="2"/>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" s="1"/>
+      <c r="B23" s="2"/>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" s="1"/>
+      <c r="B24" s="2"/>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" s="1"/>
+      <c r="B25" s="2"/>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" s="1"/>
+      <c r="B26" s="2"/>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" s="1"/>
+      <c r="B27" s="2"/>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" s="1"/>
+      <c r="B28" s="2"/>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" s="1"/>
+      <c r="B29" s="2"/>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" s="1"/>
+      <c r="B30" s="2"/>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" s="1"/>
+      <c r="B31" s="2"/>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" s="1"/>
+      <c r="B32" s="2"/>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" s="1"/>
+      <c r="B33" s="2"/>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" s="1"/>
+      <c r="B34" s="2"/>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" s="1"/>
+      <c r="B35" s="2"/>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" s="1"/>
+      <c r="B36" s="2"/>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" s="1"/>
+      <c r="B37" s="2"/>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38" s="1"/>
+      <c r="B38" s="2"/>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B39" s="2"/>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B40" s="2"/>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B41" s="2"/>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B42" s="2"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Add select data source type function #45
</commit_message>
<xml_diff>
--- a/docs/StoredVariableList.xlsx
+++ b/docs/StoredVariableList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitRepo\idep\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25FEFEFD-C341-40BA-BAE5-94B724CEEEF5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E485EDB2-FC96-4B84-B305-4B1BFC942348}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="45225" yWindow="5340" windowWidth="27000" windowHeight="14265" xr2:uid="{026807F2-CD40-4E39-BF42-D7478ABC8AA8}"/>
+    <workbookView xWindow="38280" yWindow="5145" windowWidth="29040" windowHeight="15840" xr2:uid="{026807F2-CD40-4E39-BF42-D7478ABC8AA8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
   <si>
     <t>Variable Name</t>
   </si>
@@ -72,13 +72,28 @@
   </si>
   <si>
     <t>Stage Variable: True if data is loaded.</t>
+  </si>
+  <si>
+    <t>DataSourceType</t>
+  </si>
+  <si>
+    <t>numeric</t>
+  </si>
+  <si>
+    <t>data source type:  read count / normalized expression values / Fold changes and corrected Pvalue</t>
+  </si>
+  <si>
+    <t>DataSource_noFDR</t>
+  </si>
+  <si>
+    <t>Fold-changes only, no corrected P values</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -103,6 +118,12 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -124,7 +145,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -135,6 +156,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -464,7 +486,7 @@
   <dimension ref="A1:C42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -530,12 +552,26 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="1"/>
-      <c r="B6" s="2"/>
+      <c r="A6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="1"/>
-      <c r="B7" s="2"/>
+      <c r="A7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>

</xml_diff>

<commit_message>
3rd plot is there
</commit_message>
<xml_diff>
--- a/docs/StoredVariableList.xlsx
+++ b/docs/StoredVariableList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitRepo\idep\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B0457BC-C69C-4A9D-87AF-FC7D184345F4}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62BD703F-A826-43BF-A6BF-BA06615900EE}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="5145" windowWidth="29040" windowHeight="15840" xr2:uid="{026807F2-CD40-4E39-BF42-D7478ABC8AA8}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
   <si>
     <t>Variable Name</t>
   </si>
@@ -96,6 +96,12 @@
   </si>
   <si>
     <t>return result of PreProcessing.Logic.RawDataPreprocess()</t>
+  </si>
+  <si>
+    <t>PreProcessDone</t>
+  </si>
+  <si>
+    <t>data has been pre processed</t>
   </si>
 </sst>
 </file>
@@ -495,7 +501,7 @@
   <dimension ref="A1:C42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -594,8 +600,15 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="3"/>
-      <c r="B9" s="1"/>
+      <c r="A9" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="3"/>

</xml_diff>